<commit_message>
added MME output data and figures
</commit_message>
<xml_diff>
--- a/pdfs_downscaleddata/bottom o2_thresholds.xlsx
+++ b/pdfs_downscaleddata/bottom o2_thresholds.xlsx
@@ -496,16 +496,16 @@
         <v>1.100385064871179</v>
       </c>
       <c r="D2" t="n">
-        <v>3.172380132000818</v>
+        <v>3.195530200612898</v>
       </c>
       <c r="E2" t="n">
-        <v>1.236971766849623</v>
+        <v>1.196910142261056</v>
       </c>
       <c r="F2" t="n">
-        <v>3.165496956178273</v>
+        <v>3.171945884630063</v>
       </c>
       <c r="G2" t="n">
-        <v>1.127675843754151</v>
+        <v>1.166983854326101</v>
       </c>
       <c r="H2" t="n">
         <v>3.172380132000818</v>

</xml_diff>